<commit_message>
Works whit data from db
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -454,140 +454,140 @@
         <v>GRT-1</v>
       </c>
       <c r="B2">
-        <v>131784.60647335713</v>
+        <v>131900.7940583276</v>
       </c>
       <c r="C2">
-        <v>236.3441619873047</v>
+        <v>233.8846893310547</v>
       </c>
       <c r="D2">
-        <v>229.40797424316406</v>
+        <v>233.8776092529297</v>
       </c>
       <c r="E2">
-        <v>229.56866455078125</v>
+        <v>235.66824340820312</v>
       </c>
       <c r="F2">
-        <v>69.63287353515625</v>
+        <v>52.003822326660156</v>
       </c>
       <c r="G2">
-        <v>60.33637619018555</v>
+        <v>57.20133972167969</v>
       </c>
       <c r="H2">
-        <v>61.21060562133789</v>
+        <v>52.23653793334961</v>
       </c>
       <c r="I2">
-        <v>14203.943359375</v>
+        <v>10028.87890625</v>
       </c>
       <c r="J2">
-        <v>12004.3857421875</v>
+        <v>10816.6875</v>
       </c>
       <c r="K2">
-        <v>10805.470703125</v>
+        <v>10185.5966796875</v>
       </c>
       <c r="L2">
-        <v>0.8611257076263428</v>
+        <v>0.8316212296485901</v>
       </c>
       <c r="M2">
-        <v>0.8823289275169373</v>
+        <v>0.8090195059776306</v>
       </c>
       <c r="N2">
-        <v>0.7832911610603333</v>
+        <v>0.8276892304420471</v>
       </c>
       <c r="O2">
-        <v>37505.73046875</v>
+        <v>31308.314453125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Ampak-2</v>
+        <v>Ampac-2</v>
       </c>
       <c r="B3">
-        <v>28429.661099124278</v>
+        <v>28432.502269245717</v>
       </c>
       <c r="C3">
-        <v>236.2302703857422</v>
+        <v>233.8112335205078</v>
       </c>
       <c r="D3">
-        <v>229.1161346435547</v>
+        <v>233.55409240722656</v>
       </c>
       <c r="E3">
-        <v>229.51458740234375</v>
+        <v>235.58250427246094</v>
       </c>
       <c r="F3">
-        <v>1.7833304405212402</v>
+        <v>1.158085823059082</v>
       </c>
       <c r="G3">
-        <v>1.701249122619629</v>
+        <v>1.7002322673797607</v>
       </c>
       <c r="H3">
-        <v>0.7758804559707642</v>
+        <v>2.4075684547424316</v>
       </c>
       <c r="I3">
-        <v>271.5237731933594</v>
+        <v>243.35299682617188</v>
       </c>
       <c r="J3">
-        <v>250.67672729492188</v>
+        <v>242.78810119628906</v>
       </c>
       <c r="K3">
-        <v>157.33375549316406</v>
+        <v>469.93096923828125</v>
       </c>
       <c r="L3">
-        <v>0.8669021129608154</v>
+        <v>0.8985390663146973</v>
       </c>
       <c r="M3">
-        <v>0.6447514891624451</v>
+        <v>0.6110633611679077</v>
       </c>
       <c r="N3">
-        <v>0.881385862827301</v>
+        <v>0.8282872438430786</v>
       </c>
       <c r="O3">
-        <v>679.5342407226562</v>
+        <v>956.0720825195312</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Ledena Voda-3</v>
+        <v>Ledena voda-3</v>
       </c>
       <c r="B4">
-        <v>167768.52701552786</v>
+        <v>168540.08513597416</v>
       </c>
       <c r="C4">
-        <v>213.4951934814453</v>
+        <v>234.4571533203125</v>
       </c>
       <c r="D4">
-        <v>226.35903930664062</v>
+        <v>235.22039794921875</v>
       </c>
       <c r="E4">
-        <v>222.5044708251953</v>
+        <v>236.38121032714844</v>
       </c>
       <c r="F4">
-        <v>436.1102294921875</v>
+        <v>7.332977294921875</v>
       </c>
       <c r="G4">
-        <v>453.4361267089844</v>
+        <v>8.48817253112793</v>
       </c>
       <c r="H4">
-        <v>474.055908203125</v>
+        <v>7.296930313110352</v>
       </c>
       <c r="I4">
-        <v>75415.7265625</v>
+        <v>1263.4212646484375</v>
       </c>
       <c r="J4">
-        <v>86152.40625</v>
+        <v>1575.8441162109375</v>
       </c>
       <c r="K4">
-        <v>81892.1328125</v>
+        <v>1292.468994140625</v>
       </c>
       <c r="L4">
-        <v>0.8095544576644897</v>
+        <v>0.7348595857620239</v>
       </c>
       <c r="M4">
-        <v>0.8391456604003906</v>
+        <v>0.7892672419548035</v>
       </c>
       <c r="N4">
-        <v>0.7763791680335999</v>
+        <v>0.7493193745613098</v>
       </c>
       <c r="O4">
-        <v>243460.25</v>
+        <v>4128.52978515625</v>
       </c>
     </row>
     <row r="5">
@@ -595,46 +595,46 @@
         <v>Hladilnici-4</v>
       </c>
       <c r="B5">
-        <v>125965.39631103497</v>
+        <v>126064.47047247678</v>
       </c>
       <c r="C5">
-        <v>231.41424560546875</v>
+        <v>235.95840454101562</v>
       </c>
       <c r="D5">
-        <v>229.83328247070312</v>
+        <v>234.39183044433594</v>
       </c>
       <c r="E5">
-        <v>231.0632781982422</v>
+        <v>234.66357421875</v>
       </c>
       <c r="F5">
-        <v>54.93275833129883</v>
+        <v>11.818692207336426</v>
       </c>
       <c r="G5">
-        <v>47.39447784423828</v>
+        <v>10.408903121948242</v>
       </c>
       <c r="H5">
-        <v>54.855224609375</v>
+        <v>12.592012405395508</v>
       </c>
       <c r="I5">
-        <v>10567.4033203125</v>
+        <v>2542.15771484375</v>
       </c>
       <c r="J5">
-        <v>8742.3349609375</v>
+        <v>1959.582763671875</v>
       </c>
       <c r="K5">
-        <v>10654.53125</v>
+        <v>2584.9189453125</v>
       </c>
       <c r="L5">
-        <v>0.8314470648765564</v>
+        <v>0.9115859270095825</v>
       </c>
       <c r="M5">
-        <v>0.8025659322738647</v>
+        <v>0.8031861186027527</v>
       </c>
       <c r="N5">
-        <v>0.8405923247337341</v>
+        <v>0.8747946619987488</v>
       </c>
       <c r="O5">
-        <v>29964.26953125</v>
+        <v>7090.69677734375</v>
       </c>
     </row>
     <row r="6">
@@ -642,46 +642,46 @@
         <v>Kompresorno-5</v>
       </c>
       <c r="B6">
-        <v>26766.34940923481</v>
+        <v>26854.9239010611</v>
       </c>
       <c r="C6">
-        <v>229.70201110839844</v>
+        <v>235.74732971191406</v>
       </c>
       <c r="D6">
-        <v>236.44436645507812</v>
+        <v>233.9075164794922</v>
       </c>
       <c r="E6">
-        <v>229.1887969970703</v>
+        <v>233.57058715820312</v>
       </c>
       <c r="F6">
-        <v>51.26763153076172</v>
+        <v>47.047027587890625</v>
       </c>
       <c r="G6">
-        <v>58.99839782714844</v>
+        <v>44.54290008544922</v>
       </c>
       <c r="H6">
-        <v>41.36922836303711</v>
+        <v>45.58487319946289</v>
       </c>
       <c r="I6">
-        <v>8200.24609375</v>
+        <v>8690.9462890625</v>
       </c>
       <c r="J6">
-        <v>11893.5927734375</v>
+        <v>8164.4853515625</v>
       </c>
       <c r="K6">
-        <v>7805.177734375</v>
+        <v>8207.5693359375</v>
       </c>
       <c r="L6">
-        <v>0.6928026676177979</v>
+        <v>0.7833541035652161</v>
       </c>
       <c r="M6">
-        <v>0.8504760265350342</v>
+        <v>0.7836212515830994</v>
       </c>
       <c r="N6">
-        <v>0.8222281336784363</v>
+        <v>0.7708601951599121</v>
       </c>
       <c r="O6">
-        <v>27386.806640625</v>
+        <v>25063</v>
       </c>
     </row>
     <row r="7">
@@ -689,46 +689,46 @@
         <v>Priemno-6</v>
       </c>
       <c r="B7">
-        <v>24244.817928463133</v>
+        <v>24341.95070399082</v>
       </c>
       <c r="C7">
-        <v>229.27345275878906</v>
+        <v>234.18414306640625</v>
       </c>
       <c r="D7">
-        <v>231.92196655273438</v>
+        <v>235.21852111816406</v>
       </c>
       <c r="E7">
-        <v>231.9215850830078</v>
+        <v>236.48153686523438</v>
       </c>
       <c r="F7">
-        <v>52.67059326171875</v>
+        <v>11.929794311523438</v>
       </c>
       <c r="G7">
-        <v>45.84912109375</v>
+        <v>4.372923851013184</v>
       </c>
       <c r="H7">
-        <v>47.50354766845703</v>
+        <v>3.900940418243408</v>
       </c>
       <c r="I7">
-        <v>11143.9306640625</v>
+        <v>2652.338134765625</v>
       </c>
       <c r="J7">
-        <v>9683.6943359375</v>
+        <v>588.9971923828125</v>
       </c>
       <c r="K7">
-        <v>9895.9814453125</v>
+        <v>481.669677734375</v>
       </c>
       <c r="L7">
-        <v>0.9216057062149048</v>
+        <v>0.950146496295929</v>
       </c>
       <c r="M7">
-        <v>0.9101764559745789</v>
+        <v>0.5738595128059387</v>
       </c>
       <c r="N7">
-        <v>0.8943760991096497</v>
+        <v>0.5201421976089478</v>
       </c>
       <c r="O7">
-        <v>30734.396484375</v>
+        <v>3724.3369140625</v>
       </c>
     </row>
     <row r="8">
@@ -736,46 +736,46 @@
         <v>Trafo#1-7</v>
       </c>
       <c r="B8">
-        <v>115975.72455349153</v>
+        <v>116557.51448604243</v>
       </c>
       <c r="C8">
-        <v>230.85986328125</v>
+        <v>234.64332580566406</v>
       </c>
       <c r="D8">
-        <v>230.50672912597656</v>
+        <v>234.44541931152344</v>
       </c>
       <c r="E8">
-        <v>232.5760040283203</v>
+        <v>236.64598083496094</v>
       </c>
       <c r="F8">
-        <v>321.9991149902344</v>
+        <v>33.484519958496094</v>
       </c>
       <c r="G8">
-        <v>303.5453186035156</v>
+        <v>42.40336608886719</v>
       </c>
       <c r="H8">
-        <v>327.0018310546875</v>
+        <v>38.169071197509766</v>
       </c>
       <c r="I8">
-        <v>64319.1640625</v>
+        <v>7236.0830078125</v>
       </c>
       <c r="J8">
-        <v>57757.29296875</v>
+        <v>8743.78125</v>
       </c>
       <c r="K8">
-        <v>63364.1796875</v>
+        <v>8364.05078125</v>
       </c>
       <c r="L8">
-        <v>0.8630320429801941</v>
+        <v>0.9206428527832031</v>
       </c>
       <c r="M8">
-        <v>0.8252077698707581</v>
+        <v>0.8795431852340698</v>
       </c>
       <c r="N8">
-        <v>0.8337128758430481</v>
+        <v>0.9259892702102661</v>
       </c>
       <c r="O8">
-        <v>184884.984375</v>
+        <v>24343.9140625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created new index for reading from db and getting settings from server
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -454,46 +454,46 @@
         <v>GRT-1</v>
       </c>
       <c r="B2">
-        <v>131900.7940583276</v>
+        <v>131916.49741240995</v>
       </c>
       <c r="C2">
-        <v>233.8846893310547</v>
+        <v>234.61669921875</v>
       </c>
       <c r="D2">
-        <v>233.8776092529297</v>
+        <v>235.08706665039062</v>
       </c>
       <c r="E2">
-        <v>235.66824340820312</v>
+        <v>236.3173370361328</v>
       </c>
       <c r="F2">
-        <v>52.003822326660156</v>
+        <v>9.397096633911133</v>
       </c>
       <c r="G2">
-        <v>57.20133972167969</v>
+        <v>8.64663314819336</v>
       </c>
       <c r="H2">
-        <v>52.23653793334961</v>
+        <v>7.119923114776611</v>
       </c>
       <c r="I2">
-        <v>10028.87890625</v>
+        <v>1984.673095703125</v>
       </c>
       <c r="J2">
-        <v>10816.6875</v>
+        <v>1562.0362548828125</v>
       </c>
       <c r="K2">
-        <v>10185.5966796875</v>
+        <v>1612.2728271484375</v>
       </c>
       <c r="L2">
-        <v>0.8316212296485901</v>
+        <v>0.8556978106498718</v>
       </c>
       <c r="M2">
-        <v>0.8090195059776306</v>
+        <v>0.7689777612686157</v>
       </c>
       <c r="N2">
-        <v>0.8276892304420471</v>
+        <v>0.9590601921081543</v>
       </c>
       <c r="O2">
-        <v>31308.314453125</v>
+        <v>5158.982421875</v>
       </c>
     </row>
     <row r="3">
@@ -501,46 +501,46 @@
         <v>Ampac-2</v>
       </c>
       <c r="B3">
-        <v>28432.502269245717</v>
+        <v>28434.061172639904</v>
       </c>
       <c r="C3">
-        <v>233.8112335205078</v>
+        <v>234.65138244628906</v>
       </c>
       <c r="D3">
-        <v>233.55409240722656</v>
+        <v>234.8115234375</v>
       </c>
       <c r="E3">
-        <v>235.58250427246094</v>
+        <v>236.37496948242188</v>
       </c>
       <c r="F3">
-        <v>1.158085823059082</v>
+        <v>1.0488389730453491</v>
       </c>
       <c r="G3">
-        <v>1.7002322673797607</v>
+        <v>1.7748174667358398</v>
       </c>
       <c r="H3">
-        <v>2.4075684547424316</v>
+        <v>1.5231413841247559</v>
       </c>
       <c r="I3">
-        <v>243.35299682617188</v>
+        <v>226.21859741210938</v>
       </c>
       <c r="J3">
-        <v>242.78810119628906</v>
+        <v>259.76190185546875</v>
       </c>
       <c r="K3">
-        <v>469.93096923828125</v>
+        <v>315.5941467285156</v>
       </c>
       <c r="L3">
-        <v>0.8985390663146973</v>
+        <v>0.919171154499054</v>
       </c>
       <c r="M3">
-        <v>0.6110633611679077</v>
+        <v>0.6233075261116028</v>
       </c>
       <c r="N3">
-        <v>0.8282872438430786</v>
+        <v>0.8765712976455688</v>
       </c>
       <c r="O3">
-        <v>956.0720825195312</v>
+        <v>801.5746459960938</v>
       </c>
     </row>
     <row r="4">
@@ -548,46 +548,46 @@
         <v>Ledena voda-3</v>
       </c>
       <c r="B4">
-        <v>168540.08513597416</v>
+        <v>168542.32664242078</v>
       </c>
       <c r="C4">
-        <v>234.4571533203125</v>
+        <v>234.83279418945312</v>
       </c>
       <c r="D4">
-        <v>235.22039794921875</v>
+        <v>235.4658660888672</v>
       </c>
       <c r="E4">
-        <v>236.38121032714844</v>
+        <v>236.6804962158203</v>
       </c>
       <c r="F4">
-        <v>7.332977294921875</v>
+        <v>0.2010851800441742</v>
       </c>
       <c r="G4">
-        <v>8.48817253112793</v>
+        <v>0.22693611681461334</v>
       </c>
       <c r="H4">
-        <v>7.296930313110352</v>
+        <v>0.45828041434288025</v>
       </c>
       <c r="I4">
-        <v>1263.4212646484375</v>
+        <v>31.98046112060547</v>
       </c>
       <c r="J4">
-        <v>1575.8441162109375</v>
+        <v>-17.79543113708496</v>
       </c>
       <c r="K4">
-        <v>1292.468994140625</v>
+        <v>51.478572845458984</v>
       </c>
       <c r="L4">
-        <v>0.7348595857620239</v>
+        <v>0.6772451996803284</v>
       </c>
       <c r="M4">
-        <v>0.7892672419548035</v>
+        <v>0.33302509784698486</v>
       </c>
       <c r="N4">
-        <v>0.7493193745613098</v>
+        <v>0.4746054708957672</v>
       </c>
       <c r="O4">
-        <v>4128.52978515625</v>
+        <v>65.80813598632812</v>
       </c>
     </row>
     <row r="5">
@@ -595,46 +595,46 @@
         <v>Hladilnici-4</v>
       </c>
       <c r="B5">
-        <v>126064.47047247678</v>
+        <v>126109.6145374211</v>
       </c>
       <c r="C5">
-        <v>235.95840454101562</v>
+        <v>235.8601531982422</v>
       </c>
       <c r="D5">
-        <v>234.39183044433594</v>
+        <v>234.41244506835938</v>
       </c>
       <c r="E5">
-        <v>234.66357421875</v>
+        <v>234.38795471191406</v>
       </c>
       <c r="F5">
-        <v>11.818692207336426</v>
+        <v>56.75860595703125</v>
       </c>
       <c r="G5">
-        <v>10.408903121948242</v>
+        <v>53.0229606628418</v>
       </c>
       <c r="H5">
-        <v>12.592012405395508</v>
+        <v>55.24835968017578</v>
       </c>
       <c r="I5">
-        <v>2542.15771484375</v>
+        <v>10410.4560546875</v>
       </c>
       <c r="J5">
-        <v>1959.582763671875</v>
+        <v>9372.2060546875</v>
       </c>
       <c r="K5">
-        <v>2584.9189453125</v>
+        <v>10191.412109375</v>
       </c>
       <c r="L5">
-        <v>0.9115859270095825</v>
+        <v>0.7776487469673157</v>
       </c>
       <c r="M5">
-        <v>0.8031861186027527</v>
+        <v>0.7540448904037476</v>
       </c>
       <c r="N5">
-        <v>0.8747946619987488</v>
+        <v>0.7870090007781982</v>
       </c>
       <c r="O5">
-        <v>7090.69677734375</v>
+        <v>29974.07421875</v>
       </c>
     </row>
     <row r="6">
@@ -642,46 +642,46 @@
         <v>Kompresorno-5</v>
       </c>
       <c r="B6">
-        <v>26854.9239010611</v>
+        <v>26861.310665731053</v>
       </c>
       <c r="C6">
-        <v>235.74732971191406</v>
+        <v>236.27127075195312</v>
       </c>
       <c r="D6">
-        <v>233.9075164794922</v>
+        <v>234.56773376464844</v>
       </c>
       <c r="E6">
-        <v>233.57058715820312</v>
+        <v>234.64788818359375</v>
       </c>
       <c r="F6">
-        <v>47.047027587890625</v>
+        <v>0.2897227108478546</v>
       </c>
       <c r="G6">
-        <v>44.54290008544922</v>
+        <v>0.40349316596984863</v>
       </c>
       <c r="H6">
-        <v>45.58487319946289</v>
+        <v>0.2573781907558441</v>
       </c>
       <c r="I6">
-        <v>8690.9462890625</v>
+        <v>-19.418872833251953</v>
       </c>
       <c r="J6">
-        <v>8164.4853515625</v>
+        <v>83.25874328613281</v>
       </c>
       <c r="K6">
-        <v>8207.5693359375</v>
+        <v>10.165909767150879</v>
       </c>
       <c r="L6">
-        <v>0.7833541035652161</v>
+        <v>0.28375619649887085</v>
       </c>
       <c r="M6">
-        <v>0.7836212515830994</v>
+        <v>0.8797476887702942</v>
       </c>
       <c r="N6">
-        <v>0.7708601951599121</v>
+        <v>0.16836977005004883</v>
       </c>
       <c r="O6">
-        <v>25063</v>
+        <v>74.00578308105469</v>
       </c>
     </row>
     <row r="7">
@@ -689,46 +689,46 @@
         <v>Priemno-6</v>
       </c>
       <c r="B7">
-        <v>24341.95070399082</v>
+        <v>24350.219579162927</v>
       </c>
       <c r="C7">
-        <v>234.18414306640625</v>
+        <v>234.1078643798828</v>
       </c>
       <c r="D7">
-        <v>235.21852111816406</v>
+        <v>235.02101135253906</v>
       </c>
       <c r="E7">
-        <v>236.48153686523438</v>
+        <v>236.3190155029297</v>
       </c>
       <c r="F7">
-        <v>11.929794311523438</v>
+        <v>13.248489379882812</v>
       </c>
       <c r="G7">
-        <v>4.372923851013184</v>
+        <v>4.182949066162109</v>
       </c>
       <c r="H7">
-        <v>3.900940418243408</v>
+        <v>3.9002068042755127</v>
       </c>
       <c r="I7">
-        <v>2652.338134765625</v>
+        <v>2986.270751953125</v>
       </c>
       <c r="J7">
-        <v>588.9971923828125</v>
+        <v>571.7822875976562</v>
       </c>
       <c r="K7">
-        <v>481.669677734375</v>
+        <v>479.17529296875</v>
       </c>
       <c r="L7">
-        <v>0.950146496295929</v>
+        <v>0.962823748588562</v>
       </c>
       <c r="M7">
-        <v>0.5738595128059387</v>
+        <v>0.5810154676437378</v>
       </c>
       <c r="N7">
-        <v>0.5201421976089478</v>
+        <v>0.5213376879692078</v>
       </c>
       <c r="O7">
-        <v>3724.3369140625</v>
+        <v>4049.338134765625</v>
       </c>
     </row>
     <row r="8">
@@ -736,46 +736,46 @@
         <v>Trafo#1-7</v>
       </c>
       <c r="B8">
-        <v>116557.51448604243</v>
+        <v>116594.76235985631</v>
       </c>
       <c r="C8">
-        <v>234.64332580566406</v>
+        <v>234.5697021484375</v>
       </c>
       <c r="D8">
-        <v>234.44541931152344</v>
+        <v>234.69024658203125</v>
       </c>
       <c r="E8">
-        <v>236.64598083496094</v>
+        <v>236.71922302246094</v>
       </c>
       <c r="F8">
-        <v>33.484519958496094</v>
+        <v>26.598766326904297</v>
       </c>
       <c r="G8">
-        <v>42.40336608886719</v>
+        <v>35.961387634277344</v>
       </c>
       <c r="H8">
-        <v>38.169071197509766</v>
+        <v>32.13772201538086</v>
       </c>
       <c r="I8">
-        <v>7236.0830078125</v>
+        <v>5790.56689453125</v>
       </c>
       <c r="J8">
-        <v>8743.78125</v>
+        <v>7175.96533203125</v>
       </c>
       <c r="K8">
-        <v>8364.05078125</v>
+        <v>7237.93505859375</v>
       </c>
       <c r="L8">
-        <v>0.9206428527832031</v>
+        <v>0.9280848503112793</v>
       </c>
       <c r="M8">
-        <v>0.8795431852340698</v>
+        <v>0.8502544164657593</v>
       </c>
       <c r="N8">
-        <v>0.9259892702102661</v>
+        <v>0.9514064192771912</v>
       </c>
       <c r="O8">
-        <v>24343.9140625</v>
+        <v>20204.466796875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added error handaling for the com that is right
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="23-09-2024" sheetId="1" r:id="rId1"/>
+    <sheet name="24-09-2024" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,338 +449,9 @@
         <v>Total active power</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>GRT-1</v>
-      </c>
-      <c r="B2">
-        <v>131916.49741240995</v>
-      </c>
-      <c r="C2">
-        <v>234.61669921875</v>
-      </c>
-      <c r="D2">
-        <v>235.08706665039062</v>
-      </c>
-      <c r="E2">
-        <v>236.3173370361328</v>
-      </c>
-      <c r="F2">
-        <v>9.397096633911133</v>
-      </c>
-      <c r="G2">
-        <v>8.64663314819336</v>
-      </c>
-      <c r="H2">
-        <v>7.119923114776611</v>
-      </c>
-      <c r="I2">
-        <v>1984.673095703125</v>
-      </c>
-      <c r="J2">
-        <v>1562.0362548828125</v>
-      </c>
-      <c r="K2">
-        <v>1612.2728271484375</v>
-      </c>
-      <c r="L2">
-        <v>0.8556978106498718</v>
-      </c>
-      <c r="M2">
-        <v>0.7689777612686157</v>
-      </c>
-      <c r="N2">
-        <v>0.9590601921081543</v>
-      </c>
-      <c r="O2">
-        <v>5158.982421875</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Ampac-2</v>
-      </c>
-      <c r="B3">
-        <v>28434.061172639904</v>
-      </c>
-      <c r="C3">
-        <v>234.65138244628906</v>
-      </c>
-      <c r="D3">
-        <v>234.8115234375</v>
-      </c>
-      <c r="E3">
-        <v>236.37496948242188</v>
-      </c>
-      <c r="F3">
-        <v>1.0488389730453491</v>
-      </c>
-      <c r="G3">
-        <v>1.7748174667358398</v>
-      </c>
-      <c r="H3">
-        <v>1.5231413841247559</v>
-      </c>
-      <c r="I3">
-        <v>226.21859741210938</v>
-      </c>
-      <c r="J3">
-        <v>259.76190185546875</v>
-      </c>
-      <c r="K3">
-        <v>315.5941467285156</v>
-      </c>
-      <c r="L3">
-        <v>0.919171154499054</v>
-      </c>
-      <c r="M3">
-        <v>0.6233075261116028</v>
-      </c>
-      <c r="N3">
-        <v>0.8765712976455688</v>
-      </c>
-      <c r="O3">
-        <v>801.5746459960938</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Ledena voda-3</v>
-      </c>
-      <c r="B4">
-        <v>168542.32664242078</v>
-      </c>
-      <c r="C4">
-        <v>234.83279418945312</v>
-      </c>
-      <c r="D4">
-        <v>235.4658660888672</v>
-      </c>
-      <c r="E4">
-        <v>236.6804962158203</v>
-      </c>
-      <c r="F4">
-        <v>0.2010851800441742</v>
-      </c>
-      <c r="G4">
-        <v>0.22693611681461334</v>
-      </c>
-      <c r="H4">
-        <v>0.45828041434288025</v>
-      </c>
-      <c r="I4">
-        <v>31.98046112060547</v>
-      </c>
-      <c r="J4">
-        <v>-17.79543113708496</v>
-      </c>
-      <c r="K4">
-        <v>51.478572845458984</v>
-      </c>
-      <c r="L4">
-        <v>0.6772451996803284</v>
-      </c>
-      <c r="M4">
-        <v>0.33302509784698486</v>
-      </c>
-      <c r="N4">
-        <v>0.4746054708957672</v>
-      </c>
-      <c r="O4">
-        <v>65.80813598632812</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Hladilnici-4</v>
-      </c>
-      <c r="B5">
-        <v>126109.6145374211</v>
-      </c>
-      <c r="C5">
-        <v>235.8601531982422</v>
-      </c>
-      <c r="D5">
-        <v>234.41244506835938</v>
-      </c>
-      <c r="E5">
-        <v>234.38795471191406</v>
-      </c>
-      <c r="F5">
-        <v>56.75860595703125</v>
-      </c>
-      <c r="G5">
-        <v>53.0229606628418</v>
-      </c>
-      <c r="H5">
-        <v>55.24835968017578</v>
-      </c>
-      <c r="I5">
-        <v>10410.4560546875</v>
-      </c>
-      <c r="J5">
-        <v>9372.2060546875</v>
-      </c>
-      <c r="K5">
-        <v>10191.412109375</v>
-      </c>
-      <c r="L5">
-        <v>0.7776487469673157</v>
-      </c>
-      <c r="M5">
-        <v>0.7540448904037476</v>
-      </c>
-      <c r="N5">
-        <v>0.7870090007781982</v>
-      </c>
-      <c r="O5">
-        <v>29974.07421875</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Kompresorno-5</v>
-      </c>
-      <c r="B6">
-        <v>26861.310665731053</v>
-      </c>
-      <c r="C6">
-        <v>236.27127075195312</v>
-      </c>
-      <c r="D6">
-        <v>234.56773376464844</v>
-      </c>
-      <c r="E6">
-        <v>234.64788818359375</v>
-      </c>
-      <c r="F6">
-        <v>0.2897227108478546</v>
-      </c>
-      <c r="G6">
-        <v>0.40349316596984863</v>
-      </c>
-      <c r="H6">
-        <v>0.2573781907558441</v>
-      </c>
-      <c r="I6">
-        <v>-19.418872833251953</v>
-      </c>
-      <c r="J6">
-        <v>83.25874328613281</v>
-      </c>
-      <c r="K6">
-        <v>10.165909767150879</v>
-      </c>
-      <c r="L6">
-        <v>0.28375619649887085</v>
-      </c>
-      <c r="M6">
-        <v>0.8797476887702942</v>
-      </c>
-      <c r="N6">
-        <v>0.16836977005004883</v>
-      </c>
-      <c r="O6">
-        <v>74.00578308105469</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Priemno-6</v>
-      </c>
-      <c r="B7">
-        <v>24350.219579162927</v>
-      </c>
-      <c r="C7">
-        <v>234.1078643798828</v>
-      </c>
-      <c r="D7">
-        <v>235.02101135253906</v>
-      </c>
-      <c r="E7">
-        <v>236.3190155029297</v>
-      </c>
-      <c r="F7">
-        <v>13.248489379882812</v>
-      </c>
-      <c r="G7">
-        <v>4.182949066162109</v>
-      </c>
-      <c r="H7">
-        <v>3.9002068042755127</v>
-      </c>
-      <c r="I7">
-        <v>2986.270751953125</v>
-      </c>
-      <c r="J7">
-        <v>571.7822875976562</v>
-      </c>
-      <c r="K7">
-        <v>479.17529296875</v>
-      </c>
-      <c r="L7">
-        <v>0.962823748588562</v>
-      </c>
-      <c r="M7">
-        <v>0.5810154676437378</v>
-      </c>
-      <c r="N7">
-        <v>0.5213376879692078</v>
-      </c>
-      <c r="O7">
-        <v>4049.338134765625</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Trafo#1-7</v>
-      </c>
-      <c r="B8">
-        <v>116594.76235985631</v>
-      </c>
-      <c r="C8">
-        <v>234.5697021484375</v>
-      </c>
-      <c r="D8">
-        <v>234.69024658203125</v>
-      </c>
-      <c r="E8">
-        <v>236.71922302246094</v>
-      </c>
-      <c r="F8">
-        <v>26.598766326904297</v>
-      </c>
-      <c r="G8">
-        <v>35.961387634277344</v>
-      </c>
-      <c r="H8">
-        <v>32.13772201538086</v>
-      </c>
-      <c r="I8">
-        <v>5790.56689453125</v>
-      </c>
-      <c r="J8">
-        <v>7175.96533203125</v>
-      </c>
-      <c r="K8">
-        <v>7237.93505859375</v>
-      </c>
-      <c r="L8">
-        <v>0.9280848503112793</v>
-      </c>
-      <c r="M8">
-        <v>0.8502544164657593</v>
-      </c>
-      <c r="N8">
-        <v>0.9514064192771912</v>
-      </c>
-      <c r="O8">
-        <v>20204.466796875</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>